<commit_message>
type user and admin for register and login
</commit_message>
<xml_diff>
--- a/exports/tickets.xlsx
+++ b/exports/tickets.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="92">
   <si>
     <t>Index</t>
   </si>
@@ -49,124 +49,244 @@
     <t>Created At</t>
   </si>
   <si>
-    <t>gfdb</t>
-  </si>
-  <si>
-    <t>saman.alaii10@gmail.com</t>
-  </si>
-  <si>
-    <t>ABC Inc.cx</t>
-  </si>
-  <si>
-    <t>ABCD1234</t>
-  </si>
-  <si>
-    <t>Software Bug</t>
-  </si>
-  <si>
-    <t>2023-09-03 14:30:00</t>
-  </si>
-  <si>
-    <t>Please help me with an issue.</t>
-  </si>
-  <si>
-    <t>Urgent Support Request</t>
-  </si>
-  <si>
-    <t>http://192.168.1.161:5000/uploads/1693730761718-secondimage.png</t>
-  </si>
-  <si>
-    <t>2023-09-03T08:46:01.724Z</t>
-  </si>
-  <si>
-    <t>http://192.168.1.161:5000/uploads/1693730765462-cypto-three.jpg</t>
-  </si>
-  <si>
-    <t>2023-09-03T08:46:05.480Z</t>
-  </si>
-  <si>
-    <t>http://192.168.1.161:5000/uploads/1693730767741-btcImage.webp</t>
-  </si>
-  <si>
-    <t>2023-09-03T08:46:07.746Z</t>
-  </si>
-  <si>
-    <t>http://192.168.1.161:5000/uploads/1693730772413-firstimage.png</t>
-  </si>
-  <si>
-    <t>2023-09-03T08:46:12.418Z</t>
-  </si>
-  <si>
-    <t>http://192.168.1.161:5000/uploads/1693730772980-firstimage.png</t>
-  </si>
-  <si>
-    <t>2023-09-03T08:46:12.986Z</t>
-  </si>
-  <si>
-    <t>http://192.168.1.161:5000/uploads/1693730773141-firstimage.png</t>
-  </si>
-  <si>
-    <t>2023-09-03T08:46:13.145Z</t>
-  </si>
-  <si>
-    <t>http://192.168.1.161:5000/uploads/1693730773309-firstimage.png</t>
-  </si>
-  <si>
-    <t>2023-09-03T08:46:13.313Z</t>
-  </si>
-  <si>
-    <t>http://192.168.1.161:5000/uploads/1693730773476-firstimage.png</t>
-  </si>
-  <si>
-    <t>2023-09-03T08:46:13.480Z</t>
-  </si>
-  <si>
-    <t>http://192.168.1.161:5000/uploads/1693730773656-firstimage.png</t>
-  </si>
-  <si>
-    <t>2023-09-03T08:46:13.676Z</t>
-  </si>
-  <si>
-    <t>http://192.168.1.161:5000/uploads/1693730773821-firstimage.png</t>
-  </si>
-  <si>
-    <t>2023-09-03T08:46:13.825Z</t>
-  </si>
-  <si>
-    <t>http://192.168.1.161:5000/uploads/1693730773988-firstimage.png</t>
-  </si>
-  <si>
-    <t>2023-09-03T08:46:13.992Z</t>
-  </si>
-  <si>
-    <t>http://192.168.1.161:5000/uploads/1693730774148-firstimage.png</t>
-  </si>
-  <si>
-    <t>2023-09-03T08:46:14.152Z</t>
-  </si>
-  <si>
-    <t>http://192.168.1.161:5000/uploads/1693730774316-firstimage.png</t>
-  </si>
-  <si>
-    <t>2023-09-03T08:46:14.320Z</t>
-  </si>
-  <si>
-    <t>http://192.168.1.161:5000/uploads/1693730774820-firstimage.png</t>
-  </si>
-  <si>
-    <t>2023-09-03T08:46:14.824Z</t>
-  </si>
-  <si>
-    <t>http://192.168.1.161:5000/uploads/1693730774996-firstimage.png</t>
-  </si>
-  <si>
-    <t>2023-09-03T08:46:15.000Z</t>
-  </si>
-  <si>
-    <t>http://192.168.1.161:5000/uploads/1693730775164-firstimage.png</t>
-  </si>
-  <si>
-    <t>2023-09-03T08:46:15.167Z</t>
+    <t>dvdfvdf</t>
+  </si>
+  <si>
+    <t>fvdf@gmail.com</t>
+  </si>
+  <si>
+    <t>0vdf</t>
+  </si>
+  <si>
+    <t>dfvdfvd</t>
+  </si>
+  <si>
+    <t>dvd</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720946824147-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T08:47:04.165Z</t>
+  </si>
+  <si>
+    <t>65de</t>
+  </si>
+  <si>
+    <t>sam@gmail.com</t>
+  </si>
+  <si>
+    <t>5eexde</t>
+  </si>
+  <si>
+    <t>5ee</t>
+  </si>
+  <si>
+    <t>65eed</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720947266200-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T08:54:26.203Z</t>
+  </si>
+  <si>
+    <t>wswsws</t>
+  </si>
+  <si>
+    <t>w@gmail.com</t>
+  </si>
+  <si>
+    <t>0swwswsws</t>
+  </si>
+  <si>
+    <t>swwswss</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957175813-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:39:35.823Z</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957177016-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:39:37.029Z</t>
+  </si>
+  <si>
+    <t>edwdwwdw</t>
+  </si>
+  <si>
+    <t>ede@gmail.com</t>
+  </si>
+  <si>
+    <t>wddwdwdw</t>
+  </si>
+  <si>
+    <t>dwwddw</t>
+  </si>
+  <si>
+    <t>wddwdw</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957206970-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:40:06.978Z</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957207406-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:40:07.409Z</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957207857-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:40:07.859Z</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957208302-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:40:08.305Z</t>
+  </si>
+  <si>
+    <t>swsws</t>
+  </si>
+  <si>
+    <t>s@gmail.com</t>
+  </si>
+  <si>
+    <t>swwswsws</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957236587-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:40:36.590Z</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957237023-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:40:37.025Z</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957237464-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:40:37.469Z</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957237902-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:40:37.906Z</t>
+  </si>
+  <si>
+    <t>eded</t>
+  </si>
+  <si>
+    <t>sa@gmail.com</t>
+  </si>
+  <si>
+    <t>deeded</t>
+  </si>
+  <si>
+    <t>deed</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957266240-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:41:06.245Z</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957266756-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:41:06.760Z</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957267190-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:41:07.194Z</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957267664-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:41:07.679Z</t>
+  </si>
+  <si>
+    <t>wdwdwd</t>
+  </si>
+  <si>
+    <t>wddwwd</t>
+  </si>
+  <si>
+    <t>wdwddw</t>
+  </si>
+  <si>
+    <t>wd</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957291738-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:41:31.742Z</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957292190-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:41:32.201Z</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957292640-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:41:32.670Z</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>ww@gmail.com</t>
+  </si>
+  <si>
+    <t>ujh</t>
+  </si>
+  <si>
+    <t>uj</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957328225-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:42:08.237Z</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957328725-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:42:08.730Z</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957329256-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:42:09.269Z</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/uploads/1720957329790-menu.png</t>
+  </si>
+  <si>
+    <t>2024-07-14T11:42:09.793Z</t>
   </si>
 </sst>
 </file>
@@ -543,7 +663,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L24"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -604,19 +724,19 @@
         <v>16</v>
       </c>
       <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -624,34 +744,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -659,34 +779,34 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="K4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -694,34 +814,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="J5" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="K5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -729,34 +849,34 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="I6" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="J6" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="K6" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -764,34 +884,34 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="J7" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="K7" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -799,34 +919,34 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="I8" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="J8" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="K8" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -834,34 +954,34 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="I9" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="K9" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -869,34 +989,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G10" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I10" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="J10" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="K10" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -904,34 +1024,34 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="J11" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="K11" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -939,34 +1059,34 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="H12" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I12" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="J12" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="K12" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -974,34 +1094,34 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="H13" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="I13" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="J13" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="K13" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1009,34 +1129,34 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="G14" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="H14" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="I14" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J14" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="K14" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1044,34 +1164,34 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="G15" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="H15" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="I15" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J15" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="K15" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1079,34 +1199,34 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="G16" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="H16" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="I16" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J16" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="K16" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1114,34 +1234,279 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="F17" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="G17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" t="s">
+        <v>61</v>
+      </c>
+      <c r="I17" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" t="s">
+        <v>68</v>
+      </c>
+      <c r="K17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="H17" t="s">
+      <c r="B18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" t="s">
+        <v>73</v>
+      </c>
+      <c r="J18" t="s">
+        <v>74</v>
+      </c>
+      <c r="K18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="I17" t="s">
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" t="s">
+        <v>73</v>
+      </c>
+      <c r="I19" t="s">
+        <v>73</v>
+      </c>
+      <c r="J19" t="s">
+        <v>76</v>
+      </c>
+      <c r="K19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="J17" t="s">
-        <v>50</v>
-      </c>
-      <c r="K17" t="s">
-        <v>51</v>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I20" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20" t="s">
+        <v>78</v>
+      </c>
+      <c r="K20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21" t="s">
+        <v>80</v>
+      </c>
+      <c r="H21" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" t="s">
+        <v>80</v>
+      </c>
+      <c r="J21" t="s">
+        <v>84</v>
+      </c>
+      <c r="K21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" t="s">
+        <v>80</v>
+      </c>
+      <c r="H22" t="s">
+        <v>80</v>
+      </c>
+      <c r="I22" t="s">
+        <v>80</v>
+      </c>
+      <c r="J22" t="s">
+        <v>86</v>
+      </c>
+      <c r="K22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" t="s">
+        <v>80</v>
+      </c>
+      <c r="H23" t="s">
+        <v>80</v>
+      </c>
+      <c r="I23" t="s">
+        <v>80</v>
+      </c>
+      <c r="J23" t="s">
+        <v>88</v>
+      </c>
+      <c r="K23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" t="s">
+        <v>80</v>
+      </c>
+      <c r="H24" t="s">
+        <v>80</v>
+      </c>
+      <c r="I24" t="s">
+        <v>80</v>
+      </c>
+      <c r="J24" t="s">
+        <v>90</v>
+      </c>
+      <c r="K24" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>